<commit_message>
update res mob scenario models
</commit_message>
<xml_diff>
--- a/data/residential-mobility/historical-descriptives/appendix-station-table.xlsx
+++ b/data/residential-mobility/historical-descriptives/appendix-station-table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="134">
   <si>
     <t xml:space="preserve">station_fid</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">% of in movers that are low income – CMA total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Units Built (10 year period)</t>
   </si>
   <si>
     <t xml:space="preserve">45 Street SW</t>
@@ -430,11 +433,12 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -450,12 +454,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -509,19 +507,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -542,13 +540,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.36"/>
@@ -556,7 +554,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="1" width="16.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="30.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="13" style="0" width="11.61"/>
   </cols>
@@ -592,25 +590,28 @@
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>0.484304932735426</v>
@@ -630,19 +631,19 @@
         <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0.431266846361186</v>
@@ -662,19 +663,19 @@
         <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0.579288025889968</v>
@@ -694,19 +695,19 @@
         <v>26</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>0.690140845070423</v>
@@ -726,19 +727,19 @@
         <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>0.579406631762653</v>
@@ -758,19 +759,19 @@
         <v>33</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>0.49476135040745</v>
@@ -790,19 +791,19 @@
         <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>0.748366013071895</v>
@@ -822,22 +823,22 @@
         <v>36</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>0.665885378786877</v>
@@ -854,19 +855,19 @@
         <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>0.700325732899023</v>
@@ -886,22 +887,22 @@
         <v>47</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>0.665885378786877</v>
@@ -918,19 +919,19 @@
         <v>50</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="n">
         <v>0.81701030927835</v>
@@ -950,19 +951,19 @@
         <v>57</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>0.951668092386655</v>
@@ -982,19 +983,19 @@
         <v>60</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>0.63953488372093</v>
@@ -1014,19 +1015,19 @@
         <v>61</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>0.75098814229249</v>
@@ -1046,19 +1047,19 @@
         <v>63</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G16" s="1" t="n">
         <v>0.467032967032967</v>
@@ -1078,22 +1079,22 @@
         <v>64</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>0.693946835946501</v>
@@ -1110,22 +1111,22 @@
         <v>67</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>0.665885378786877</v>
@@ -1142,19 +1143,19 @@
         <v>69</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G19" s="1" t="n">
         <v>0.64897466827503</v>
@@ -1174,22 +1175,22 @@
         <v>72</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>0.665885378786877</v>
@@ -1206,19 +1207,19 @@
         <v>73</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G21" s="1" t="n">
         <v>0.620220900594732</v>
@@ -1238,22 +1239,22 @@
         <v>80</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>0.653851289092698</v>
@@ -1270,22 +1271,22 @@
         <v>81</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>0.653851289092698</v>
@@ -1302,19 +1303,19 @@
         <v>82</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G24" s="1" t="n">
         <v>0.802127659574468</v>
@@ -1334,19 +1335,19 @@
         <v>138</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G25" s="1" t="n">
         <v>0.83355091383812</v>
@@ -1366,19 +1367,19 @@
         <v>141</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="G26" s="1" t="n">
         <v>0.765432098765432</v>
@@ -1398,19 +1399,19 @@
         <v>144</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G27" s="1" t="n">
         <v>0.75417439703154</v>
@@ -1430,22 +1431,22 @@
         <v>148</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>0.604914336093498</v>
@@ -1462,19 +1463,19 @@
         <v>186</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G29" s="1" t="n">
         <v>0.817527010804322</v>
@@ -1494,22 +1495,22 @@
         <v>197</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>0.612311755251334</v>
@@ -1526,22 +1527,22 @@
         <v>224</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>0.595809967591091</v>
@@ -1558,19 +1559,19 @@
         <v>266</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G32" s="1" t="n">
         <v>0.733228097868982</v>
@@ -1590,22 +1591,22 @@
         <v>267</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H33" s="1" t="n">
         <v>0.591465183806798</v>
@@ -1622,19 +1623,19 @@
         <v>286</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>0.745409015025042</v>
@@ -1654,22 +1655,22 @@
         <v>298</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H35" s="1" t="n">
         <v>0.604914336093498</v>
@@ -1686,22 +1687,22 @@
         <v>311</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H36" s="1" t="n">
         <v>0.586399396054801</v>
@@ -1718,19 +1719,19 @@
         <v>346</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>0.552356020942408</v>
@@ -1750,22 +1751,22 @@
         <v>383</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H38" s="1" t="n">
         <v>0.718211797045227</v>
@@ -1782,19 +1783,19 @@
         <v>393</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G39" s="1" t="n">
         <v>0.454380390376759</v>
@@ -1814,19 +1815,19 @@
         <v>485</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>0.489239598278336</v>
@@ -1846,19 +1847,19 @@
         <v>486</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F41" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>90</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>0.518763796909492</v>
@@ -1878,22 +1879,22 @@
         <v>499</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="D42" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H42" s="1" t="n">
         <v>0.544947136496101</v>
@@ -1910,19 +1911,19 @@
         <v>652</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G43" s="1" t="n">
         <v>0.699119911991199</v>
@@ -1942,19 +1943,19 @@
         <v>656</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F44" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="G44" s="1" t="n">
         <v>0.767175572519084</v>
@@ -1974,19 +1975,19 @@
         <v>657</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G45" s="1" t="n">
         <v>0.485304659498208</v>
@@ -2006,19 +2007,19 @@
         <v>658</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G46" s="1" t="n">
         <v>0.635771543086172</v>
@@ -2038,19 +2039,19 @@
         <v>659</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G47" s="1" t="n">
         <v>0.715736040609137</v>
@@ -2070,19 +2071,19 @@
         <v>668</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G48" s="1" t="n">
         <v>0.837658017298736</v>
@@ -2102,19 +2103,19 @@
         <v>673</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G49" s="1" t="n">
         <v>0.698250728862974</v>
@@ -2134,19 +2135,19 @@
         <v>674</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G50" s="1" t="n">
         <v>0.868175765645806</v>
@@ -2166,19 +2167,19 @@
         <v>676</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G51" s="1" t="n">
         <v>0.612903225806452</v>
@@ -2198,19 +2199,19 @@
         <v>678</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G52" s="1" t="n">
         <v>0.915523465703971</v>
@@ -2230,19 +2231,19 @@
         <v>680</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G53" s="1" t="n">
         <v>0.446145723336853</v>
@@ -2262,19 +2263,19 @@
         <v>682</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G54" s="1" t="n">
         <v>0.415671117357695</v>
@@ -2294,19 +2295,19 @@
         <v>683</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G55" s="1" t="n">
         <v>0.868680999418942</v>
@@ -2326,22 +2327,22 @@
         <v>686</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H56" s="1" t="n">
         <v>0.687846997020971</v>
@@ -2358,19 +2359,19 @@
         <v>687</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G57" s="1" t="n">
         <v>0.431077694235589</v>
@@ -2390,22 +2391,22 @@
         <v>689</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H58" s="1" t="n">
         <v>0.687846997020971</v>
@@ -2422,19 +2423,19 @@
         <v>694</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G59" s="1" t="n">
         <v>0.462387853692202</v>
@@ -2454,19 +2455,19 @@
         <v>695</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G60" s="1" t="n">
         <v>0.824429865666979</v>
@@ -2486,19 +2487,19 @@
         <v>696</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G61" s="1" t="n">
         <v>0.768693918245264</v>
@@ -2518,22 +2519,22 @@
         <v>698</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H62" s="1" t="n">
         <v>0.687846997020971</v>
@@ -2550,19 +2551,19 @@
         <v>699</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G63" s="1" t="n">
         <v>0.6640625</v>
@@ -2582,19 +2583,19 @@
         <v>700</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G64" s="1" t="n">
         <v>0.639312977099237</v>
@@ -2614,19 +2615,19 @@
         <v>702</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G65" s="1" t="n">
         <v>0.767491926803014</v>
@@ -2646,19 +2647,19 @@
         <v>703</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G66" s="1" t="n">
         <v>0.521933500977927</v>
@@ -2678,19 +2679,19 @@
         <v>705</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G67" s="1" t="n">
         <v>0.724400871459695</v>
@@ -2710,19 +2711,19 @@
         <v>710</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G68" s="1" t="n">
         <v>0.72198275862069</v>
@@ -2742,19 +2743,19 @@
         <v>714</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G69" s="1" t="n">
         <v>0.527696793002916</v>
@@ -2774,19 +2775,19 @@
         <v>715</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G70" s="1" t="n">
         <v>0.858993229319988</v>
@@ -2806,19 +2807,19 @@
         <v>718</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G71" s="1" t="n">
         <v>0.519191460367931</v>

</xml_diff>